<commit_message>
Align text of birthdays
</commit_message>
<xml_diff>
--- a/Empregados.xlsx
+++ b/Empregados.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ravin\Desktop\send_email_python\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ravin\Desktop\send_email_coletivo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEC99122-3B05-466A-907D-2EB7D7CD762B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D90AA6D4-611B-43CB-A6C8-0C966625A190}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{652DF72A-66DF-46A1-927A-2A14980F385E}"/>
   </bookViews>
   <sheets>
-    <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="DataBase" sheetId="1" r:id="rId1"/>
+    <sheet name="Assinatura" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4166" uniqueCount="2108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4171" uniqueCount="2113">
   <si>
     <t>Str_Mat_Outlook</t>
   </si>
@@ -6357,13 +6358,28 @@
   </si>
   <si>
     <t>YURI RYOKI GOMES SUKIYAMA AREDES</t>
+  </si>
+  <si>
+    <t>Assinatura</t>
+  </si>
+  <si>
+    <t>SR Brasília sul</t>
+  </si>
+  <si>
+    <t>marciano.matos@caixa.gov.br</t>
+  </si>
+  <si>
+    <t>Superintendente de Rede</t>
+  </si>
+  <si>
+    <t>Marciano de Freitas Matos</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -6371,16 +6387,36 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -6388,13 +6424,29 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6743,8 +6795,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98547958-D657-46E7-B850-726EE50AB189}">
   <dimension ref="A1:J1040"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7287,7 +7339,7 @@
         <v>1410</v>
       </c>
       <c r="E17" s="1">
-        <v>21192</v>
+        <v>21212</v>
       </c>
       <c r="F17" s="1">
         <v>39146</v>
@@ -40050,25 +40102,50 @@
 </worksheet>
 </file>
 
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAF5A61D-A000-4249-A437-2513555A6A21}">
+  <dimension ref="A1:A5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>2108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>2112</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>2109</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>2110</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>2111</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100AABFCBE3A081344CBD19FDD7D36B97EC" ma:contentTypeVersion="13" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="65b3017dae72f3457fbfe08cdcab5d5b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns3="fa4d580a-d01a-42c3-9b98-e13a85c10f62" xmlns:ns4="874b114b-9a7e-49de-8627-5ddbce6c662f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e26fdd407132aebd9a4b758b3c93b41b" ns1:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -40294,25 +40371,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2BF6B064-3CDA-4685-9D85-ED77979C9B22}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF7D4AB7-832D-4E2C-B10A-11961EB6AB4B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AEA40C47-9E4B-43D8-AED4-0A7727DB5564}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -40330,4 +40407,22 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF7D4AB7-832D-4E2C-B10A-11961EB6AB4B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2BF6B064-3CDA-4685-9D85-ED77979C9B22}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Create function ExistingDayOfTheWeek to be used in the message
</commit_message>
<xml_diff>
--- a/Empregados.xlsx
+++ b/Empregados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ravin\Desktop\send_email_coletivo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D90AA6D4-611B-43CB-A6C8-0C966625A190}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{219CA7B5-6B52-44AA-83E0-E5FB8A2F820C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{652DF72A-66DF-46A1-927A-2A14980F385E}"/>
   </bookViews>
@@ -6796,7 +6796,7 @@
   <dimension ref="A1:J1040"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6859,7 +6859,7 @@
         <v>1586</v>
       </c>
       <c r="E2" s="1">
-        <v>17902</v>
+        <v>17925</v>
       </c>
       <c r="F2" s="1">
         <v>38698</v>
@@ -6891,7 +6891,7 @@
         <v>817</v>
       </c>
       <c r="E3" s="1">
-        <v>18911</v>
+        <v>18655</v>
       </c>
       <c r="F3" s="1">
         <v>43752</v>
@@ -7307,7 +7307,7 @@
         <v>638</v>
       </c>
       <c r="E16" s="1">
-        <v>21177</v>
+        <v>20847</v>
       </c>
       <c r="F16" s="1">
         <v>29731</v>
@@ -32203,7 +32203,7 @@
         <v>797</v>
       </c>
       <c r="E794" s="1">
-        <v>31804</v>
+        <v>31794</v>
       </c>
       <c r="F794" s="1">
         <v>41435</v>

</xml_diff>

<commit_message>
Adjust proportional align with much people birthday
</commit_message>
<xml_diff>
--- a/Empregados.xlsx
+++ b/Empregados.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ravin\Desktop\send_email_coletivo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arthur\Desktop\workspace\send_leyman_email_coletivo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{219CA7B5-6B52-44AA-83E0-E5FB8A2F820C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AC2CDA7-71D1-4D76-89EB-6F64F971E80E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{652DF72A-66DF-46A1-927A-2A14980F385E}"/>
   </bookViews>
@@ -6795,8 +6795,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98547958-D657-46E7-B850-726EE50AB189}">
   <dimension ref="A1:J1040"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="C661" workbookViewId="0">
+      <selection activeCell="E663" sqref="E663"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6859,7 +6859,7 @@
         <v>1586</v>
       </c>
       <c r="E2" s="1">
-        <v>17925</v>
+        <v>17902</v>
       </c>
       <c r="F2" s="1">
         <v>38698</v>
@@ -6891,7 +6891,7 @@
         <v>817</v>
       </c>
       <c r="E3" s="1">
-        <v>18655</v>
+        <v>18911</v>
       </c>
       <c r="F3" s="1">
         <v>43752</v>
@@ -7307,7 +7307,7 @@
         <v>638</v>
       </c>
       <c r="E16" s="1">
-        <v>20847</v>
+        <v>21177</v>
       </c>
       <c r="F16" s="1">
         <v>29731</v>
@@ -7339,7 +7339,7 @@
         <v>1410</v>
       </c>
       <c r="E17" s="1">
-        <v>21212</v>
+        <v>21192</v>
       </c>
       <c r="F17" s="1">
         <v>39146</v>
@@ -25387,10 +25387,10 @@
         <v>698</v>
       </c>
       <c r="E581" s="1">
-        <v>30091</v>
+        <v>30090</v>
       </c>
       <c r="F581" s="1">
-        <v>42142</v>
+        <v>42979</v>
       </c>
       <c r="G581">
         <v>2272</v>
@@ -25419,10 +25419,10 @@
         <v>265</v>
       </c>
       <c r="E582" s="1">
-        <v>30098</v>
+        <v>30090</v>
       </c>
       <c r="F582" s="1">
-        <v>44400</v>
+        <v>42979</v>
       </c>
       <c r="G582">
         <v>3872</v>
@@ -25451,10 +25451,10 @@
         <v>1105</v>
       </c>
       <c r="E583" s="1">
-        <v>30099</v>
+        <v>30090</v>
       </c>
       <c r="F583" s="1">
-        <v>41498</v>
+        <v>42979</v>
       </c>
       <c r="G583">
         <v>643</v>
@@ -25483,10 +25483,10 @@
         <v>1562</v>
       </c>
       <c r="E584" s="1">
-        <v>30112</v>
+        <v>30090</v>
       </c>
       <c r="F584" s="1">
-        <v>40371</v>
+        <v>39881</v>
       </c>
       <c r="G584">
         <v>674</v>
@@ -25515,10 +25515,10 @@
         <v>614</v>
       </c>
       <c r="E585" s="1">
-        <v>30113</v>
+        <v>30090</v>
       </c>
       <c r="F585" s="1">
-        <v>41085</v>
+        <v>39118</v>
       </c>
       <c r="G585">
         <v>1057</v>
@@ -25547,10 +25547,10 @@
         <v>1229</v>
       </c>
       <c r="E586" s="1">
-        <v>30132</v>
+        <v>39881</v>
       </c>
       <c r="F586" s="1">
-        <v>37935</v>
+        <v>39118</v>
       </c>
       <c r="G586">
         <v>8</v>
@@ -25579,10 +25579,10 @@
         <v>598</v>
       </c>
       <c r="E587" s="1">
-        <v>30137</v>
+        <v>39881</v>
       </c>
       <c r="F587" s="1">
-        <v>39881</v>
+        <v>39118</v>
       </c>
       <c r="G587">
         <v>3697</v>
@@ -25611,7 +25611,7 @@
         <v>1231</v>
       </c>
       <c r="E588" s="1">
-        <v>30139</v>
+        <v>39881</v>
       </c>
       <c r="F588" s="1">
         <v>39118</v>
@@ -28043,7 +28043,7 @@
         <v>476</v>
       </c>
       <c r="E664" s="1">
-        <v>30648</v>
+        <v>30751</v>
       </c>
       <c r="F664" s="1">
         <v>38754</v>
@@ -28075,7 +28075,7 @@
         <v>901</v>
       </c>
       <c r="E665" s="1">
-        <v>30664</v>
+        <v>30751</v>
       </c>
       <c r="F665" s="1">
         <v>40518</v>
@@ -28107,7 +28107,7 @@
         <v>1761</v>
       </c>
       <c r="E666" s="1">
-        <v>30670</v>
+        <v>30751</v>
       </c>
       <c r="F666" s="1">
         <v>39545</v>
@@ -28139,7 +28139,7 @@
         <v>1277</v>
       </c>
       <c r="E667" s="1">
-        <v>30697</v>
+        <v>30751</v>
       </c>
       <c r="F667" s="1">
         <v>41680</v>
@@ -28171,7 +28171,7 @@
         <v>855</v>
       </c>
       <c r="E668" s="1">
-        <v>30703</v>
+        <v>30752</v>
       </c>
       <c r="F668" s="1">
         <v>40637</v>
@@ -28203,7 +28203,7 @@
         <v>1345</v>
       </c>
       <c r="E669" s="1">
-        <v>30725</v>
+        <v>30752</v>
       </c>
       <c r="F669" s="1">
         <v>43773</v>
@@ -28235,7 +28235,7 @@
         <v>1915</v>
       </c>
       <c r="E670" s="1">
-        <v>30728</v>
+        <v>30752</v>
       </c>
       <c r="F670" s="1">
         <v>41323</v>
@@ -28267,7 +28267,7 @@
         <v>825</v>
       </c>
       <c r="E671" s="1">
-        <v>30729</v>
+        <v>30752</v>
       </c>
       <c r="F671" s="1">
         <v>41498</v>
@@ -28299,7 +28299,7 @@
         <v>1989</v>
       </c>
       <c r="E672" s="1">
-        <v>30741</v>
+        <v>30752</v>
       </c>
       <c r="F672" s="1">
         <v>43972</v>
@@ -28331,7 +28331,7 @@
         <v>200</v>
       </c>
       <c r="E673" s="1">
-        <v>30743</v>
+        <v>30752</v>
       </c>
       <c r="F673" s="1">
         <v>43752</v>
@@ -28363,7 +28363,7 @@
         <v>622</v>
       </c>
       <c r="E674" s="1">
-        <v>30744</v>
+        <v>30752</v>
       </c>
       <c r="F674" s="1">
         <v>41953</v>
@@ -28395,7 +28395,7 @@
         <v>1365</v>
       </c>
       <c r="E675" s="1">
-        <v>30746</v>
+        <v>30752</v>
       </c>
       <c r="F675" s="1">
         <v>43658</v>
@@ -28427,7 +28427,7 @@
         <v>738</v>
       </c>
       <c r="E676" s="1">
-        <v>30750</v>
+        <v>30752</v>
       </c>
       <c r="F676" s="1">
         <v>40917</v>
@@ -32203,7 +32203,7 @@
         <v>797</v>
       </c>
       <c r="E794" s="1">
-        <v>31794</v>
+        <v>31804</v>
       </c>
       <c r="F794" s="1">
         <v>41435</v>
@@ -40146,6 +40146,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100AABFCBE3A081344CBD19FDD7D36B97EC" ma:contentTypeVersion="13" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="65b3017dae72f3457fbfe08cdcab5d5b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns3="fa4d580a-d01a-42c3-9b98-e13a85c10f62" xmlns:ns4="874b114b-9a7e-49de-8627-5ddbce6c662f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e26fdd407132aebd9a4b758b3c93b41b" ns1:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -40371,7 +40380,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -40380,16 +40389,17 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2BF6B064-3CDA-4685-9D85-ED77979C9B22}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AEA40C47-9E4B-43D8-AED4-0A7727DB5564}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -40409,20 +40419,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF7D4AB7-832D-4E2C-B10A-11961EB6AB4B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2BF6B064-3CDA-4685-9D85-ED77979C9B22}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>